<commit_message>
Improve string/value conversion. Test unicode handling.
svn:1185 7b1320e8-e022-0410-a07a-c339c07ae202
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr saveExternalLinkValues="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="195" windowWidth="11010" windowHeight="6630" tabRatio="250"/>
+    <workbookView xWindow="675" yWindow="195" windowWidth="11010" windowHeight="6630" tabRatio="250" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Box Int array" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>eiij asj</t>
   </si>
   <si>
-    <t>eiij</t>
-  </si>
-  <si>
     <t>Lorem</t>
   </si>
   <si>
@@ -52,15 +49,23 @@
   <si>
     <t>ad Augusta</t>
   </si>
+  <si>
+    <t>鳴箏金粟柱</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +391,7 @@
   </sheetPr>
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -1203,7 +1209,9 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -1216,8 +1224,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1235,13 +1243,13 @@
       <c r="A4">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.75" footer="0.75"/>
-  <pageSetup paperSize="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -2091,16 +2099,16 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
       </c>
       <c r="G3">
         <v>24</v>
@@ -2120,16 +2128,16 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
       <c r="E4">
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>33</v>
@@ -2149,16 +2157,16 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>39</v>
       </c>
       <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
         <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
       </c>
       <c r="G5">
         <v>42</v>
@@ -2178,16 +2186,16 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
       </c>
       <c r="G6">
         <v>51</v>

</xml_diff>

<commit_message>
Add tests for some number formats. Add first draft of xslt using `general/pcall/disp` syntax.
svn:1189 7b1320e8-e022-0410-a07a-c339c07ae202
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr saveExternalLinkValues="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="195" windowWidth="11010" windowHeight="6630" tabRatio="250" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="675" yWindow="195" windowWidth="11010" windowHeight="6630" tabRatio="250" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Box Int array" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Box Mix array" sheetId="3" r:id="rId3"/>
     <sheet name="Offset" sheetId="4" r:id="rId4"/>
     <sheet name="Diff Mix array" sheetId="5" r:id="rId5"/>
+    <sheet name="Number Fmt" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -88,9 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,7 +1211,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2272,4 +2274,63 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="6" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2">
+        <v>50000</v>
+      </c>
+      <c r="C1" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D1" s="2">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="E1" s="2">
+        <v>500000000</v>
+      </c>
+      <c r="F1" s="2">
+        <v>500000000.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>-5</v>
+      </c>
+      <c r="B2">
+        <v>-50000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-4.9999999999999998E-7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-500000000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-500000000.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>